<commit_message>
final N-policy linking plots
</commit_message>
<xml_diff>
--- a/Plotting/production_shares_ammonia_LowAmbition.xlsx
+++ b/Plotting/production_shares_ammonia_LowAmbition.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,20 @@
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration_1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -496,6 +510,36 @@
           <t>2050</t>
         </is>
       </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>2040</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>2040</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -504,13 +548,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1183999.999999999</v>
+        <v>1184000.000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>4954.489800842347</v>
+        <v>4810.151102347427</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.620644115050832e-10</v>
+        <v>-2.620601923793058e-10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1184000.000000074</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1183999.999999876</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -523,10 +585,28 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1175338.318472064</v>
+        <v>1175482.441022393</v>
       </c>
       <c r="D5" t="n">
-        <v>1180233.186001361</v>
+        <v>1180214.184748082</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +622,25 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>52.26682757255812</v>
+        <v>71.29135345365613</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1181739.817836299</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1181730.993934782</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.984140500134267e-07</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1181737.653169923</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1181730.993934819</v>
       </c>
     </row>
     <row r="7">
@@ -560,6 +658,24 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6.694979318452933e-09</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -576,6 +692,24 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -592,6 +726,24 @@
       <c r="D9" t="n">
         <v>0</v>
       </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -608,6 +760,24 @@
       <c r="D10" t="n">
         <v>0</v>
       </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -624,6 +794,24 @@
       <c r="D11" t="n">
         <v>0</v>
       </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -640,6 +828,24 @@
       <c r="D12" t="n">
         <v>0</v>
       </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -656,6 +862,24 @@
       <c r="D13" t="n">
         <v>0</v>
       </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -672,6 +896,24 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -688,10 +930,30 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
+    <mergeCell ref="H1:J1"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>